<commit_message>
found sources for district heat and electricity use in PJ
</commit_message>
<xml_diff>
--- a/scenario_data/scenario_data.xlsx
+++ b/scenario_data/scenario_data.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="34">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -126,7 +126,7 @@
     <t xml:space="preserve">production|district heat|Excess from fuels</t>
   </si>
   <si>
-    <t xml:space="preserve">production|district heat|District heat use</t>
+    <t xml:space="preserve">consumption|district heat|District heat use</t>
   </si>
   <si>
     <t xml:space="preserve">lossess|district heat|distribution losses</t>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumption|electricity|residential electricity use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gwh</t>
   </si>
 </sst>
 </file>
@@ -181,18 +187,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -246,7 +246,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -286,10 +286,10 @@
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A20"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="59.48"/>
   </cols>
@@ -807,10 +807,10 @@
         <v>11</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>-0.0199728</v>
+        <v>74.2</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>-0.0217872</v>
+        <v>68.8</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -879,14 +879,30 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>8394</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>7724.71</v>
+      </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>

</xml_diff>

<commit_message>
defined pathways and markets for indidual heat and electricity
</commit_message>
<xml_diff>
--- a/scenario_data/scenario_data.xlsx
+++ b/scenario_data/scenario_data.xlsx
@@ -25,7 +25,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="E18" authorId="0">
+    <comment ref="E21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -139,28 +139,28 @@
     <t xml:space="preserve">production|district heat|Excess from fuels</t>
   </si>
   <si>
+    <t xml:space="preserve">lossess|district heat|distribution losses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lossess|electricity|distribution losses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumption|electricity|residential electricity use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gwh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumption|individual heat|individual heat use</t>
+  </si>
+  <si>
     <t xml:space="preserve">consumption|district heat|District heat use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lossess|district heat|distribution losses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lossess|electricity|distribution losses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">consumption|electricity|residential electricity use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gwh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">consumption|individual heat|individual heat use</t>
   </si>
 </sst>
 </file>
@@ -245,7 +245,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -256,10 +256,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -299,13 +295,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="59.48"/>
   </cols>
@@ -816,17 +812,19 @@
       <c r="D18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>27</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>74.2</v>
+        <f aca="false">1/0.2</f>
+        <v>5</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>68.8</v>
+        <f aca="false">1/0.2</f>
+        <v>5</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -846,18 +844,18 @@
         <v>9</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G19" s="2" t="n">
-        <f aca="false">1/0.2</f>
-        <v>5</v>
+        <f aca="false">1/0.7</f>
+        <v>1.42857142857143</v>
       </c>
       <c r="H19" s="2" t="n">
-        <f aca="false">1/0.2</f>
-        <v>5</v>
+        <f aca="false">1/0.7</f>
+        <v>1.42857142857143</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -876,19 +874,17 @@
       <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>30</v>
+      <c r="E20" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G20" s="2" t="n">
-        <f aca="false">1/0.7</f>
-        <v>1.42857142857143</v>
+        <v>8394</v>
       </c>
       <c r="H20" s="2" t="n">
-        <f aca="false">1/0.7</f>
-        <v>1.42857142857143</v>
+        <v>7724.71</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -907,17 +903,17 @@
       <c r="D21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>32</v>
+      <c r="E21" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>8394</v>
+        <v>53.7</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>7724.71</v>
+        <v>70.1</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -936,17 +932,17 @@
       <c r="D22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>53.7</v>
+        <v>74.2</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>70.1</v>
+        <v>68.8</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -957,7 +953,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="3"/>
       <c r="F23" s="1"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -970,7 +966,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="4"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -998,8 +994,8 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -1011,30 +1007,20 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1"/>
@@ -1050,91 +1036,88 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="7"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1"/>
-      <c r="J36" s="6"/>
+      <c r="E36" s="7"/>
+      <c r="J36" s="5"/>
       <c r="K36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1"/>
-      <c r="E37" s="8"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="7"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1"/>
       <c r="J38" s="6"/>
-      <c r="K38" s="7"/>
+      <c r="K38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="1"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="1"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="7"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="1"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="7"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="1"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
+      <c r="E43" s="7"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1"/>
-      <c r="E44" s="8"/>
+      <c r="E44" s="7"/>
       <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
+      <c r="K44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="1"/>
-      <c r="E45" s="8"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="6"/>
+      <c r="E45" s="7"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="1"/>
-      <c r="E46" s="8"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="6"/>
+      <c r="E46" s="7"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="1"/>
-      <c r="E47" s="8"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="1"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
changed to kwh and mj
</commit_message>
<xml_diff>
--- a/scenario_data/scenario_data.xlsx
+++ b/scenario_data/scenario_data.xlsx
@@ -25,7 +25,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="E21" authorId="0">
+    <comment ref="E23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -38,7 +38,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0">
+    <comment ref="E24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="38">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -91,73 +91,82 @@
     <t xml:space="preserve">production|individual heat|solar heat</t>
   </si>
   <si>
+    <t xml:space="preserve">MJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|individual heat|air heat pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|individual heat|ground heat pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|individual heat|biomass furnace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|individual heat|biomass stove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|individual heat|biomass pellets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|individual heat|sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|district heat|Woodchips CHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|district heat|Gas CHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|district heat|Waste CHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|district heat|Biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|district heat|heat pumps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|district heat|Geothermal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|district heat|Solar heat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|district heat|Residual industrial heat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|district heat|Wood boiler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|district heat|Straw boiler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production|district heat|Excess from fuels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lossess|district heat|distribution losses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lossess|electricity|distribution losses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumption|electricity|residential electricity use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumption|individual heat|individual heat use</t>
+  </si>
+  <si>
     <t xml:space="preserve">PJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|individual heat|air heat pump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|individual heat|ground heat pump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|individual heat|biomass furnace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|individual heat|sum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|district heat|Woodchips CHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|district heat|Gas CHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|district heat|Waste CHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|district heat|Biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|district heat|heat pumps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|district heat|Geothermal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|district heat|Solar heat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|district heat|Residual industrial heat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|district heat|Wood boiler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|district heat|Straw boiler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production|district heat|Excess from fuels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lossess|district heat|distribution losses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lossess|electricity|distribution losses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">consumption|electricity|residential electricity use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gwh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">consumption|individual heat|individual heat use</t>
   </si>
   <si>
     <t xml:space="preserve">consumption|district heat|District heat use</t>
@@ -203,12 +212,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -245,7 +260,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -256,6 +271,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -295,15 +318,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A192" activeCellId="0" sqref="A192"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="59.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="17.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -355,13 +379,13 @@
         <v>11</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+        <v>2500000000</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>5000000000</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,13 +408,13 @@
         <v>11</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>12.6</v>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>3.9564</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+        <v>12600000000</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>3956400000</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,42 +437,42 @@
         <v>11</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>37.9215</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>54.657</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+        <v>37921500000</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>54657000000</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>25.17048</v>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>0.1008</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+        <v>25170480000</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>26170480000</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,13 +495,13 @@
         <v>11</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>78.19198</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>63.7142</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+        <v>12585240000</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>13085240000</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,13 +524,13 @@
         <v>11</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+        <v>12585240000</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>13085240000</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -522,20 +546,20 @@
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>10.24488</v>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>4.87728</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+        <v>78191980000</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>63714200000</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,20 +575,20 @@
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>27.379944</v>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>29.4804</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
       <c r="K9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,20 +604,20 @@
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>21.4760484</v>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+        <v>10244880000</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>4877280000</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
       <c r="K10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,20 +633,20 @@
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>11.18664</v>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>17.82054</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+        <v>27379944000</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>29480400000</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -638,20 +662,20 @@
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>4.75236</v>
-      </c>
-      <c r="H12" s="2" t="n">
-        <v>4.19004</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+        <v>21476048400</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -667,20 +691,20 @@
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="H13" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+        <v>11186640000</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>17820540000</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -696,20 +720,20 @@
       <c r="D14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+        <v>4752360000</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>4190040000</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,20 +749,20 @@
       <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+        <v>3500000000</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>7000000000</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,20 +778,20 @@
       <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>22.19868</v>
-      </c>
-      <c r="H16" s="2" t="n">
-        <v>7.5582</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+        <v>4700000000</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>4700000000</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,7 +807,7 @@
       <c r="D17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -792,11 +816,11 @@
       <c r="G17" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="H17" s="2" t="n">
-        <v>0.0032472</v>
-      </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="H17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,79 +836,77 @@
       <c r="D18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>22198680000</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>7558200000</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="F19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>3247200</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="2" t="n">
         <f aca="false">1/0.2</f>
         <v>5</v>
       </c>
-      <c r="H18" s="2" t="n">
+      <c r="H20" s="2" t="n">
         <f aca="false">1/0.2</f>
         <v>5</v>
-      </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="2" t="n">
-        <f aca="false">1/0.7</f>
-        <v>1.42857142857143</v>
-      </c>
-      <c r="H19" s="2" t="n">
-        <f aca="false">1/0.7</f>
-        <v>1.42857142857143</v>
-      </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20" s="2" t="n">
-        <v>8394</v>
-      </c>
-      <c r="H20" s="2" t="n">
-        <v>7724.71</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -903,17 +925,19 @@
       <c r="D21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>33</v>
+      <c r="E21" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>53.7</v>
+        <f aca="false">1/0.7</f>
+        <v>1.42857142857143</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>70.1</v>
+        <f aca="false">1/0.7</f>
+        <v>1.42857142857143</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -932,44 +956,76 @@
       <c r="D22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="G22" s="2" t="n">
-        <v>74.2</v>
+        <v>8394000</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>68.8</v>
+        <v>7724710</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="A23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>53700000000</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>70100000000</v>
+      </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="A24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>74200000000</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>68800000000</v>
+      </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -979,7 +1035,7 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="5"/>
       <c r="F25" s="1"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -994,8 +1050,8 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -1014,16 +1070,36 @@
       <c r="K27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
       <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="1"/>
@@ -1036,88 +1112,94 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1"/>
-      <c r="E36" s="7"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="6"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="6"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
+      <c r="E38" s="9"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="1"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="6"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="1"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="6"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="1"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="1"/>
-      <c r="E43" s="7"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1"/>
-      <c r="E44" s="7"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="5"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="1"/>
-      <c r="E45" s="7"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="5"/>
+      <c r="E45" s="9"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="1"/>
-      <c r="E46" s="7"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
+      <c r="E46" s="9"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="1"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
+      <c r="E47" s="9"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
+      <c r="E48" s="9"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="1"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="1"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fixed decimal errors and units for electricity
</commit_message>
<xml_diff>
--- a/scenario_data/scenario_data.xlsx
+++ b/scenario_data/scenario_data.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="37">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t xml:space="preserve">consumption|individual heat|individual heat use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PJ</t>
   </si>
   <si>
     <t xml:space="preserve">consumption|district heat|District heat use</t>
@@ -176,12 +173,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.00"/>
-    <numFmt numFmtId="167" formatCode="#,##0"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="167" formatCode="0"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
+    <numFmt numFmtId="169" formatCode="#,##0"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -260,7 +259,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -289,11 +288,19 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -321,7 +328,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -963,13 +970,13 @@
         <v>34</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>8394000</v>
+        <v>8394000000</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>7724710</v>
-      </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+        <v>7724710000</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -989,7 +996,7 @@
         <v>35</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>53700000000</v>
@@ -997,8 +1004,8 @@
       <c r="H23" s="2" t="n">
         <v>70100000000</v>
       </c>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
       <c r="K23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,10 +1022,10 @@
         <v>9</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="G24" s="2" t="n">
         <v>74200000000</v>
@@ -1026,8 +1033,8 @@
       <c r="H24" s="2" t="n">
         <v>68800000000</v>
       </c>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
       <c r="K24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1037,10 +1044,10 @@
       <c r="D25" s="1"/>
       <c r="E25" s="5"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
       <c r="K25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,8 +1083,8 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -1118,88 +1125,88 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="8"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1"/>
-      <c r="E38" s="9"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="8"/>
+      <c r="E38" s="11"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="10"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="8"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="10"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="1"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="1"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="1"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="8"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="10"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="1"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="8"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="10"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="1"/>
-      <c r="E45" s="9"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
+      <c r="E45" s="11"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="1"/>
-      <c r="E46" s="9"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="7"/>
+      <c r="E46" s="11"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="9"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="1"/>
-      <c r="E47" s="9"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="7"/>
+      <c r="E47" s="11"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1"/>
-      <c r="E48" s="9"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
+      <c r="E48" s="11"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="1"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="1"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>